<commit_message>
v0.8: improved excel loading. fixed missing pi and other fields
</commit_message>
<xml_diff>
--- a/src/already_requested_metadata.xlsx
+++ b/src/already_requested_metadata.xlsx
@@ -8,38 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\data-metadata\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{57EB6CFD-E80B-438A-AEAA-012B702C57AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7258E01-FE65-453F-9D73-752FCFA11288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="1350" windowWidth="21600" windowHeight="12530" xr2:uid="{B1986E0D-1066-4DF6-B073-1EB572532559}"/>
+    <workbookView xWindow="6160" yWindow="2370" windowWidth="19130" windowHeight="10610" activeTab="1" xr2:uid="{B1986E0D-1066-4DF6-B073-1EB572532559}"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="ADIDO Metadata" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
-  <si>
-    <t>report</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>classification</t>
-  </si>
-  <si>
-    <t>pi</t>
-  </si>
-  <si>
-    <t>pci</t>
-  </si>
-  <si>
-    <t>treatment</t>
-  </si>
-  <si>
     <t>report_1</t>
   </si>
   <si>
@@ -74,6 +60,30 @@
   </si>
   <si>
     <t>rounded</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Field Name</t>
+  </si>
+  <si>
+    <t>Business Description</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>PCI</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>not available</t>
+  </si>
+  <si>
+    <t>Data Treatment</t>
   </si>
 </sst>
 </file>
@@ -933,194 +943,244 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E010385B-8CF0-4E41-A099-A2F7B812E58C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E77966A-E7E9-4204-A016-12AC6F116326}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>